<commit_message>
New-JohnstrupUsers.psm1 Added Remove-JohnstrupUsers Tested ok.
BrugeradmSDmenu.ps1
jonstrupned tilføjet til menu

JohnstrupNedlæggelseFraExcel.ps1
First commit. Tested ok.

JohnstrupOprettelseFraExcel.ps1
Changed approver NALH to EVAL
Company option is now number shortcuts, instead od fist letter in name.
Fixed remove-item path to the new path varible.
$FileName to $FilePath
</commit_message>
<xml_diff>
--- a/PS_scripts/TestBrugerJonstrup.xlsx
+++ b/PS_scripts/TestBrugerJonstrup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jebn\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RUFR_PowerShell\PS_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -394,7 +394,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +442,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="5">
-        <v>9999900</v>
+        <v>9999910</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>26</v>
@@ -465,7 +465,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="5">
-        <v>9999903</v>
+        <v>9999911</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>26</v>
@@ -485,7 +485,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="5">
-        <v>9999902</v>
+        <v>9999912</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>26</v>
@@ -505,7 +505,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="5">
-        <v>9999904</v>
+        <v>9999913</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>26</v>
@@ -525,7 +525,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="5">
-        <v>9999901</v>
+        <v>9999914</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>26</v>
@@ -545,7 +545,7 @@
         <v>21</v>
       </c>
       <c r="D7" s="5">
-        <v>9999905</v>
+        <v>9999915</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>26</v>
@@ -565,7 +565,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="5">
-        <v>9999906</v>
+        <v>9999916</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>26</v>
@@ -585,7 +585,7 @@
         <v>25</v>
       </c>
       <c r="D9" s="5">
-        <v>9999907</v>
+        <v>9999917</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>26</v>
@@ -597,7 +597,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E4:E10" r:id="rId2" display="test@mail.sletmig"/>
+    <hyperlink ref="E4:E9" r:id="rId2" display="test@mail.sletmig"/>
     <hyperlink ref="E7" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
PSADT and Packages examples
</commit_message>
<xml_diff>
--- a/PS_scripts/TestBrugerJonstrup.xlsx
+++ b/PS_scripts/TestBrugerJonstrup.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RUFR_PowerShell\PS_scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalData\RUFR_PowerShell\PS_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11F8BEE-81FF-48D2-988C-0658FD2A8A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -110,7 +111,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,7 +158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -167,12 +168,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -390,25 +388,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="F2" sqref="F2:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" customWidth="1"/>
+    <col min="4" max="4" width="35.26953125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.1796875" customWidth="1"/>
+    <col min="6" max="6" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -431,7 +429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -441,20 +439,17 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="3">
         <v>9999910</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="F2">
-        <v>41273324</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -464,17 +459,15 @@
       <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>9999911</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="3">
-        <v>27548735</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -484,17 +477,14 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>9999912</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F4">
-        <v>42337760</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -504,17 +494,15 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>9999913</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="3">
-        <v>21473142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -524,17 +512,15 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>9999914</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="3">
-        <v>29849595</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -544,17 +530,15 @@
       <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>9999915</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="3">
-        <v>42545426</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -564,17 +548,15 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="3">
         <v>9999916</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="3">
-        <v>60516919</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -584,21 +566,19 @@
       <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <v>9999917</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="3">
-        <v>53621809</v>
-      </c>
+      <c r="F9" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E4:E9" r:id="rId2" display="test@mail.sletmig"/>
-    <hyperlink ref="E7" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E4:E9" r:id="rId2" display="test@mail.sletmig" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>